<commit_message>
update index.html, contents and feedback page
</commit_message>
<xml_diff>
--- a/contents/battle_1/battle_1.xlsx
+++ b/contents/battle_1/battle_1.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3C93CE-FE92-4D25-8436-94445417B166}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86651A5D-E0EE-4C39-9B5B-57D45557B0E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="10620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
     <sheet name="interactions" sheetId="2" r:id="rId2"/>
     <sheet name="units" sheetId="3" r:id="rId3"/>
+    <sheet name="parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="57">
   <si>
     <t>x</t>
   </si>
@@ -71,9 +72,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>attack</t>
-  </si>
-  <si>
     <t>defense</t>
   </si>
   <si>
@@ -162,6 +160,45 @@
   </si>
   <si>
     <t>towers</t>
+  </si>
+  <si>
+    <t>siege</t>
+  </si>
+  <si>
+    <t>attack_melee</t>
+  </si>
+  <si>
+    <t>attack_range</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>melee_distance</t>
+  </si>
+  <si>
+    <t>melee_height_difference_threshold</t>
+  </si>
+  <si>
+    <t>archer_distance</t>
+  </si>
+  <si>
+    <t>archer_distance_height_gain</t>
+  </si>
+  <si>
+    <t>siege_distance</t>
+  </si>
+  <si>
+    <t>siege_distance_height_gain</t>
+  </si>
+  <si>
+    <t>flier_distance</t>
+  </si>
+  <si>
+    <t>flier_distance_height_gain</t>
   </si>
 </sst>
 </file>
@@ -194,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +286,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -262,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,12 +319,18 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -559,7 +608,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>9</v>
@@ -630,7 +679,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>9</v>
@@ -650,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>9</v>
@@ -670,7 +719,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>9</v>
@@ -690,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>9</v>
@@ -710,10 +759,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -730,10 +779,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -750,10 +799,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -770,10 +819,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -790,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -810,10 +859,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -830,10 +879,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>9</v>
@@ -853,7 +902,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>9</v>
@@ -873,10 +922,10 @@
         <v>1</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>9</v>
@@ -896,7 +945,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -913,10 +962,10 @@
         <v>2</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>9</v>
@@ -936,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>9</v>
@@ -950,16 +999,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>15.5</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>9</v>
@@ -973,37 +1022,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A63502-AF7A-4054-B79C-125248EE72B4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="11">
         <v>2</v>
@@ -1011,12 +1063,12 @@
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="11">
         <v>2</v>
@@ -1024,12 +1076,12 @@
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="11">
         <v>2</v>
@@ -1037,12 +1089,12 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="11">
         <v>-1</v>
@@ -1052,12 +1104,12 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="11">
         <v>-1</v>
@@ -1067,18 +1119,18 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
@@ -1089,12 +1141,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9">
         <v>-1</v>
@@ -1108,20 +1160,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35488FFD-9895-4BA3-BA35-EBF213FD10A0}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
@@ -1135,598 +1189,746 @@
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>4</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
       <c r="I4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>33</v>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>33</v>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>32</v>
+      <c r="C7" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>6</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
+      <c r="C8" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>7</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
       <c r="J8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
-        <v>32</v>
+      <c r="C9" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>8</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
       <c r="J9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
+      <c r="C10" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>9</v>
       </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
       <c r="J10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
-        <v>32</v>
+      <c r="C11" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>10</v>
       </c>
-      <c r="I11">
-        <v>2</v>
-      </c>
       <c r="J11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
-        <v>32</v>
+      <c r="C12" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
         <v>4</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>11</v>
       </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
       <c r="J12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" t="s">
-        <v>34</v>
+      <c r="C13" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>5</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>12</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
       <c r="J13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
-        <v>32</v>
+      <c r="C14" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
         <v>4</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>13</v>
       </c>
-      <c r="I14">
-        <v>2</v>
-      </c>
       <c r="J14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" t="s">
-        <v>34</v>
+      <c r="C15" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
         <v>5</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>14</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
       <c r="J15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
-        <v>34</v>
+      <c r="C16" s="13" t="s">
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
         <v>5</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>15</v>
       </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
       <c r="J16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>5</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>16</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
       <c r="J17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
-        <v>35</v>
+      <c r="C18" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>5</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>17</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
       <c r="J18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
-        <v>23</v>
-      </c>
       <c r="E19">
         <v>3</v>
       </c>
       <c r="F19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
         <v>12</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>18</v>
       </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
       <c r="J19">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1402C5AC-6BA8-4199-9EF0-F087CEA6081F}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>